<commit_message>
Did a lot of documentation
</commit_message>
<xml_diff>
--- a/doc/thesis/pictures/resultate/loesung2/variante2/resultate_median.xlsx
+++ b/doc/thesis/pictures/resultate/loesung2/variante2/resultate_median.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView minimized="1" xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -775,11 +775,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="299745744"/>
-        <c:axId val="299747704"/>
+        <c:axId val="255136240"/>
+        <c:axId val="255137024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="299745744"/>
+        <c:axId val="255136240"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -903,13 +903,13 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299747704"/>
+        <c:crossAx val="255137024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="299747704"/>
+        <c:axId val="255137024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1022,7 +1022,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299745744"/>
+        <c:crossAx val="255136240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -2016,8 +2016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>